<commit_message>
AUTO FROM HOME 06.05.2024 22:36:50,62
</commit_message>
<xml_diff>
--- a/Дудкин/Книга1.xlsx
+++ b/Дудкин/Книга1.xlsx
@@ -13,6 +13,10 @@
   </sheets>
   <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -264,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,6 +323,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -624,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,17 +648,11 @@
         <f>B1*A1</f>
         <v>4.8</v>
       </c>
-      <c r="H1">
-        <v>84.3</v>
-      </c>
-      <c r="I1">
-        <v>87.89</v>
-      </c>
-      <c r="K1">
-        <v>0.76</v>
-      </c>
-      <c r="L1">
-        <v>0.76</v>
+      <c r="E1">
+        <v>540.92999999999995</v>
+      </c>
+      <c r="F1">
+        <v>542.72075000000007</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -665,16 +666,14 @@
         <f t="shared" ref="C2:C32" si="0">B2*A2</f>
         <v>4.5</v>
       </c>
-      <c r="H2" s="17">
-        <v>52.48</v>
-      </c>
-      <c r="I2">
-        <f>38.14+11.18</f>
-        <v>49.32</v>
-      </c>
-      <c r="Q2" s="18">
-        <v>1.78</v>
-      </c>
+      <c r="E2">
+        <v>611.2509</v>
+      </c>
+      <c r="F2">
+        <v>613.27444750000006</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -687,15 +686,13 @@
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
-      <c r="H3">
-        <v>1814.4</v>
-      </c>
-      <c r="I3">
-        <v>1834.56</v>
-      </c>
-      <c r="Q3" s="19">
-        <v>22.09</v>
-      </c>
+      <c r="E3">
+        <v>207.82530600000001</v>
+      </c>
+      <c r="F3">
+        <v>208.51331215000005</v>
+      </c>
+      <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -708,17 +705,15 @@
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-      <c r="H4">
-        <v>0.46</v>
-      </c>
-      <c r="I4">
-        <v>0.48</v>
-      </c>
-      <c r="Q4" s="19">
-        <v>7.51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>87.6</v>
+      </c>
+      <c r="F4" s="20">
+        <v>87.89</v>
+      </c>
+      <c r="Q4" s="19"/>
+    </row>
+    <row r="5" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -729,15 +724,14 @@
         <f t="shared" si="0"/>
         <v>1.58</v>
       </c>
-      <c r="H5">
-        <v>5.52</v>
-      </c>
-      <c r="I5">
-        <v>5.28</v>
-      </c>
-      <c r="Q5" s="19">
-        <v>0.19</v>
-      </c>
+      <c r="E5">
+        <v>11.18</v>
+      </c>
+      <c r="F5" s="17">
+        <f xml:space="preserve"> 0.39*(87.89*0.4+0.29*0.35)</f>
+        <v>13.750425</v>
+      </c>
+      <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -750,15 +744,13 @@
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
-      <c r="H6">
-        <v>600.64</v>
-      </c>
-      <c r="I6">
-        <v>540.92999999999995</v>
-      </c>
-      <c r="Q6" s="19">
-        <v>68.42</v>
-      </c>
+      <c r="E6">
+        <v>38.14</v>
+      </c>
+      <c r="F6" s="20">
+        <v>38.14</v>
+      </c>
+      <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -771,21 +763,14 @@
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-      <c r="H7" s="17">
-        <v>1801.92</v>
-      </c>
-      <c r="I7">
-        <f>350*540.93/100</f>
-        <v>1893.2549999999997</v>
-      </c>
-      <c r="N7">
-        <f>49.32/3652.4</f>
-        <v>1.3503449786441791E-2</v>
-      </c>
-      <c r="Q7">
-        <f>SUM(Q2:Q6)</f>
-        <v>99.990000000000009</v>
-      </c>
+      <c r="E7">
+        <v>49.32</v>
+      </c>
+      <c r="F7">
+        <f>F6+F5</f>
+        <v>51.890425</v>
+      </c>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
@@ -798,21 +783,14 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8">
-        <v>684.73</v>
-      </c>
-      <c r="I8">
-        <v>611.25</v>
+      <c r="E8" s="17">
+        <v>2766.94</v>
+      </c>
+      <c r="F8" s="17">
+        <f xml:space="preserve"> 51.89+ 613.27+208.51+5.28+1899.52</f>
+        <v>2778.47</v>
       </c>
       <c r="L8" s="17"/>
-      <c r="N8">
-        <f>1893.26/2766.94*100</f>
-        <v>68.424324343859993</v>
-      </c>
-      <c r="Q8">
-        <f>11.18/3652.4</f>
-        <v>3.061000985653269E-3</v>
-      </c>
     </row>
     <row r="9" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
@@ -825,22 +803,16 @@
         <f t="shared" si="0"/>
         <v>13.200000000000001</v>
       </c>
-      <c r="H9">
-        <v>232.81</v>
-      </c>
-      <c r="I9" s="17">
-        <v>207.83</v>
-      </c>
-      <c r="N9">
-        <f>5.28/2766.94*100</f>
-        <v>0.19082452095094221</v>
-      </c>
-      <c r="Q9">
-        <f>2766.94/3652.4</f>
-        <v>0.75756762676596212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1893.26</v>
+      </c>
+      <c r="F9">
+        <f>350*F1/100</f>
+        <v>1899.5226250000001</v>
+      </c>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -851,19 +823,15 @@
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
-      <c r="H10">
-        <v>2777.46</v>
-      </c>
-      <c r="I10">
-        <f>49.32+ 611.25+207.83+5.28+1893.255</f>
-        <v>2766.9350000000004</v>
-      </c>
-      <c r="N10">
-        <f>2016*91/100</f>
-        <v>1834.56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="17">
+        <v>3043.63</v>
+      </c>
+      <c r="F10" s="17">
+        <f xml:space="preserve"> 2778.5 + 277.85</f>
+        <v>3056.35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>4</v>
       </c>
@@ -874,19 +842,15 @@
         <f t="shared" si="0"/>
         <v>6.8</v>
       </c>
-      <c r="H11">
-        <v>3055</v>
-      </c>
-      <c r="I11">
-        <f>2766.94 + 276.69</f>
-        <v>3043.63</v>
-      </c>
-      <c r="N11">
-        <f>87.89/N10</f>
-        <v>4.7907945229373805E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="17">
+        <v>608.73</v>
+      </c>
+      <c r="F11">
+        <f>3056.4/5</f>
+        <v>611.28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>1</v>
       </c>
@@ -897,18 +861,15 @@
         <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
-      <c r="H12">
-        <v>611</v>
-      </c>
-      <c r="I12">
-        <v>608.73</v>
-      </c>
-      <c r="N12">
-        <f>350*540.93/100</f>
-        <v>1893.2549999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="17">
+        <v>3652.4</v>
+      </c>
+      <c r="F12" s="17">
+        <f xml:space="preserve"> 3056.4+611.28</f>
+        <v>3667.6800000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11">
         <v>5</v>
       </c>
@@ -919,18 +880,15 @@
         <f t="shared" si="0"/>
         <v>5.3000000000000007</v>
       </c>
-      <c r="H13">
-        <v>3666</v>
-      </c>
-      <c r="I13">
-        <v>3652.4</v>
-      </c>
-      <c r="N13">
-        <f>20*3043.63/100</f>
-        <v>608.72600000000011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F13">
+        <f>F7/F12</f>
+        <v>1.4148024091523796E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -941,15 +899,12 @@
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="H14">
-        <v>1.89</v>
-      </c>
-      <c r="I14">
-        <v>1.78</v>
-      </c>
-      <c r="N14">
-        <f>1100*0.048/10</f>
-        <v>5.28</v>
+      <c r="E14" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="F14">
+        <f>F5/F12*100</f>
+        <v>0.37490797997644287</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -963,16 +918,14 @@
         <f t="shared" si="0"/>
         <v>2.0999999999999996</v>
       </c>
-      <c r="H15">
-        <v>24.65</v>
-      </c>
-      <c r="I15">
-        <v>22.09</v>
-      </c>
-      <c r="N15" s="17">
-        <f xml:space="preserve"> 3043.63+608.73</f>
-        <v>3652.36</v>
-      </c>
+      <c r="E15" s="17">
+        <v>0.76</v>
+      </c>
+      <c r="F15">
+        <f>F8/F12</f>
+        <v>0.75755518474894201</v>
+      </c>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -985,18 +938,8 @@
         <f t="shared" si="0"/>
         <v>4.8999999999999995</v>
       </c>
-      <c r="H16">
-        <v>8.3800000000000008</v>
-      </c>
-      <c r="I16">
-        <v>7.51</v>
-      </c>
-      <c r="N16">
-        <f>611.25/2766.94*100</f>
-        <v>22.091190990769586</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -1007,18 +950,8 @@
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="H17">
-        <v>0.2</v>
-      </c>
-      <c r="I17">
-        <v>0.19</v>
-      </c>
-      <c r="O17">
-        <f>49.32/2766.94*100</f>
-        <v>1.7824745025190283</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>7</v>
       </c>
@@ -1029,18 +962,8 @@
         <f t="shared" si="0"/>
         <v>2.0299999999999998</v>
       </c>
-      <c r="H18">
-        <v>64.87</v>
-      </c>
-      <c r="I18">
-        <v>68.42</v>
-      </c>
-      <c r="N18">
-        <f>207.86/2766.94*100</f>
-        <v>7.5122698721331149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>5</v>
       </c>
@@ -1051,14 +974,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I19">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>1</v>
       </c>
@@ -1069,14 +986,8 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H20">
-        <v>10.72</v>
-      </c>
-      <c r="I20">
-        <v>11.18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -1087,14 +998,8 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H21">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I21">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>1</v>
       </c>
@@ -1106,7 +1011,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>6</v>
       </c>
@@ -1118,7 +1023,7 @@
         <v>2.4000000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -1130,7 +1035,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>1</v>
       </c>
@@ -1142,7 +1047,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>3</v>
       </c>
@@ -1154,7 +1059,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>1</v>
       </c>
@@ -1166,7 +1071,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>4</v>
       </c>
@@ -1178,7 +1083,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>5</v>
       </c>
@@ -1190,7 +1095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>3</v>
       </c>
@@ -1202,7 +1107,7 @@
         <v>1.7399999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -1214,7 +1119,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>105</v>
       </c>

</xml_diff>